<commit_message>
Add students info and make special events P/F.
</commit_message>
<xml_diff>
--- a/PySparkExample/Data/StudentInfo.xlsx
+++ b/PySparkExample/Data/StudentInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github_ndsu\CSCI422Misc\PySparkExample\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2127CEDD-8095-4EF3-BB69-138797C6688F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4D5844-ACE5-446E-9E9B-974EA1BE3019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25180" windowHeight="16140" xr2:uid="{80FB1615-3458-49F1-B8B3-2E1F8BCCBC04}"/>
+    <workbookView xWindow="20" yWindow="740" windowWidth="24940" windowHeight="15900" xr2:uid="{80FB1615-3458-49F1-B8B3-2E1F8BCCBC04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -396,18 +396,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208139BE-0131-4A73-93BB-0AC678A42BDB}">
-  <dimension ref="A1:C41"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49:C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -418,7 +418,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -428,23 +428,23 @@
       </c>
       <c r="C2" t="str">
         <f ca="1">IF(RAND()&lt;0.5, "North Dakota", IF(RAND()&lt;0.7, "Minnesota", IF(RAND()&lt;0.8, "Montana", "Other")))</f>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B41" ca="1" si="0">IF(RAND()&lt;0.8, "Computer Science", IF(RAND()&gt;0.5, "Computer Engineering", "Other"))</f>
+        <f t="shared" ref="B3:B51" ca="1" si="0">IF(RAND()&lt;0.8, "Computer Science", IF(RAND()&gt;0.5, "Computer Engineering", "Other"))</f>
         <v>Computer Science</v>
       </c>
       <c r="C3" t="str">
-        <f t="shared" ref="C3:C41" ca="1" si="1">IF(RAND()&lt;0.5, "North Dakota", IF(RAND()&lt;0.7, "Minnesota", IF(RAND()&lt;0.8, "Montana", "Other")))</f>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <f t="shared" ref="C3:C51" ca="1" si="1">IF(RAND()&lt;0.5, "North Dakota", IF(RAND()&lt;0.7, "Minnesota", IF(RAND()&lt;0.8, "Montana", "Other")))</f>
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -454,36 +454,36 @@
       </c>
       <c r="C4" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Montana</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Computer Engineering</v>
+        <v>Computer Science</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Minnesota</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Computer Science</v>
+        <v>Computer Engineering</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>North Dakota</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -493,10 +493,10 @@
       </c>
       <c r="C7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Other</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -509,7 +509,7 @@
         <v>North Dakota</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -519,23 +519,23 @@
       </c>
       <c r="C9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>North Dakota</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Computer Science</v>
+        <v>Other</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Minnesota</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -548,20 +548,20 @@
         <v>Minnesota</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Computer Engineering</v>
+        <v>Computer Science</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -571,23 +571,23 @@
       </c>
       <c r="C13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Montana</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Computer Science</v>
+        <v>Computer Engineering</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>North Dakota</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -597,10 +597,10 @@
       </c>
       <c r="C15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Montana</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -613,7 +613,7 @@
         <v>North Dakota</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -623,10 +623,10 @@
       </c>
       <c r="C17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -636,23 +636,23 @@
       </c>
       <c r="C18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Computer Science</v>
+        <v>Other</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>North Dakota</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Montana</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -662,23 +662,23 @@
       </c>
       <c r="C20" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>North Dakota</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Computer Science</v>
+        <v>Computer Engineering</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>North Dakota</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -691,7 +691,7 @@
         <v>North Dakota</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -701,10 +701,10 @@
       </c>
       <c r="C23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Other</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -714,10 +714,10 @@
       </c>
       <c r="C24" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>North Dakota</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -730,7 +730,7 @@
         <v>North Dakota</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -740,23 +740,23 @@
       </c>
       <c r="C26" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>North Dakota</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Montana</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Other</v>
+        <v>Computer Engineering</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" ca="1" si="1"/>
         <v>Minnesota</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -769,20 +769,20 @@
         <v>North Dakota</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Other</v>
+        <v>Computer Science</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>North Dakota</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -795,7 +795,7 @@
         <v>Minnesota</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -805,10 +805,10 @@
       </c>
       <c r="C31" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Montana</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -818,23 +818,23 @@
       </c>
       <c r="C32" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>North Dakota</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Montana</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Computer Science</v>
+        <v>Other</v>
       </c>
       <c r="C33" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>North Dakota</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -844,10 +844,10 @@
       </c>
       <c r="C34" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -857,10 +857,10 @@
       </c>
       <c r="C35" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -870,10 +870,10 @@
       </c>
       <c r="C36" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>North Dakota</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -883,23 +883,23 @@
       </c>
       <c r="C37" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>Computer Engineering</v>
+        <v>Computer Science</v>
       </c>
       <c r="C38" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Minnesota</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>38</v>
       </c>
@@ -912,7 +912,7 @@
         <v>Minnesota</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>39</v>
       </c>
@@ -922,20 +922,150 @@
       </c>
       <c r="C40" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>Montana</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" ca="1" si="0"/>
+        <v>Computer Science</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Computer Science</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Computer Science</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Computer Science</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Computer Science</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" ca="1" si="1"/>
         <v>Other</v>
       </c>
-      <c r="C41" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>Montana</v>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Computer Science</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Other</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Computer Science</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>North Dakota</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Computer Engineering</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Computer Science</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Minnesota</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>Computer Science</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>North Dakota</v>
       </c>
     </row>
   </sheetData>

</xml_diff>